<commit_message>
change test scenario name in test scenario
</commit_message>
<xml_diff>
--- a/ScenarioTest_finalweb.xlsx
+++ b/ScenarioTest_finalweb.xlsx
@@ -260,9 +260,6 @@
     <t>PRODUCT</t>
   </si>
   <si>
-    <t>Add rating</t>
-  </si>
-  <si>
     <t>3. Click image product</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>success add rating</t>
+  </si>
+  <si>
+    <t>WP-3  Winda - Add rating</t>
   </si>
 </sst>
 </file>
@@ -725,13 +725,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -740,25 +746,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -785,6 +782,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1009,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" workbookViewId="0">
       <selection activeCell="C36" sqref="C36:C43"/>
     </sheetView>
   </sheetViews>
@@ -1031,22 +1031,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
+      <c r="B1" s="50"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="48" t="s">
+      <c r="F1" s="50"/>
+      <c r="G1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="49"/>
+      <c r="H1" s="48"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1101,22 +1101,22 @@
       <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="51"/>
+      <c r="B3" s="50"/>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="53" t="s">
+      <c r="F3" s="50"/>
+      <c r="G3" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="49"/>
+      <c r="H3" s="48"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -1169,15 +1169,15 @@
       <c r="AB4" s="3"/>
     </row>
     <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="51"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="55" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1217,7 +1217,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="57"/>
+      <c r="E6" s="56"/>
       <c r="F6" s="10">
         <v>1</v>
       </c>
@@ -1378,10 +1378,10 @@
       <c r="C11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="55"/>
+      <c r="E11" s="54"/>
       <c r="F11" s="18" t="s">
         <v>18</v>
       </c>
@@ -1415,13 +1415,13 @@
       <c r="AB11" s="3"/>
     </row>
     <row r="12" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="43" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="25" t="s">
@@ -1435,7 +1435,7 @@
       <c r="H12" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="45" t="s">
+      <c r="I12" s="36" t="s">
         <v>11</v>
       </c>
       <c r="J12" s="2"/>
@@ -1459,9 +1459,9 @@
       <c r="AB12" s="3"/>
     </row>
     <row r="13" spans="1:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="43"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="22" t="s">
         <v>32</v>
       </c>
@@ -1473,7 +1473,7 @@
       <c r="H13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="46"/>
+      <c r="I13" s="37"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -1495,9 +1495,9 @@
       <c r="AB13" s="3"/>
     </row>
     <row r="14" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="37"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="43"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="22" t="s">
         <v>33</v>
       </c>
@@ -1509,7 +1509,7 @@
       <c r="H14" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="46"/>
+      <c r="I14" s="37"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -1531,9 +1531,9 @@
       <c r="AB14" s="3"/>
     </row>
     <row r="15" spans="1:28" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="37"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="43"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="21" t="s">
         <v>35</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
-      <c r="I15" s="46"/>
+      <c r="I15" s="37"/>
       <c r="J15" s="4"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1565,9 +1565,9 @@
       <c r="AB15" s="3"/>
     </row>
     <row r="16" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="44"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="27" t="s">
         <v>34</v>
       </c>
@@ -1579,7 +1579,7 @@
       <c r="H16" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1592,11 +1592,11 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="42" t="s">
+      <c r="B17" s="42"/>
+      <c r="C17" s="43" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="25" t="s">
@@ -1610,7 +1610,7 @@
       <c r="H17" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="45" t="s">
+      <c r="I17" s="36" t="s">
         <v>11</v>
       </c>
       <c r="J17" s="3"/>
@@ -1625,9 +1625,9 @@
       <c r="S17" s="3"/>
     </row>
     <row r="18" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="43"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="22" t="s">
         <v>32</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="H18" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="46"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1652,9 +1652,9 @@
       <c r="S18" s="3"/>
     </row>
     <row r="19" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="43"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="22" t="s">
         <v>33</v>
       </c>
@@ -1666,7 +1666,7 @@
       <c r="H19" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="46"/>
+      <c r="I19" s="37"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1679,9 +1679,9 @@
       <c r="S19" s="3"/>
     </row>
     <row r="20" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="43"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="21" t="s">
         <v>35</v>
       </c>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="46"/>
+      <c r="I20" s="37"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1704,9 +1704,9 @@
       <c r="S20" s="3"/>
     </row>
     <row r="21" spans="1:19" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="38"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="44"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="27" t="s">
         <v>34</v>
       </c>
@@ -1718,7 +1718,7 @@
       <c r="H21" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="I21" s="47"/>
+      <c r="I21" s="38"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1731,13 +1731,13 @@
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="43" t="s">
         <v>44</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -1751,7 +1751,7 @@
       <c r="H22" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="45" t="s">
+      <c r="I22" s="36" t="s">
         <v>12</v>
       </c>
       <c r="J22" s="3"/>
@@ -1766,9 +1766,9 @@
       <c r="S22" s="3"/>
     </row>
     <row r="23" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="37"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="43"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="22" t="s">
         <v>32</v>
       </c>
@@ -1780,7 +1780,7 @@
       <c r="H23" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="I23" s="46"/>
+      <c r="I23" s="37"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -1793,9 +1793,9 @@
       <c r="S23" s="3"/>
     </row>
     <row r="24" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="43"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="22" t="s">
         <v>45</v>
       </c>
@@ -1807,7 +1807,7 @@
       <c r="H24" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="I24" s="46"/>
+      <c r="I24" s="37"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -1820,9 +1820,9 @@
       <c r="S24" s="3"/>
     </row>
     <row r="25" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="43"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="21" t="s">
         <v>47</v>
       </c>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
-      <c r="I25" s="46"/>
+      <c r="I25" s="37"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -1845,9 +1845,9 @@
       <c r="S25" s="3"/>
     </row>
     <row r="26" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="38"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="44"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="27" t="s">
         <v>48</v>
       </c>
@@ -1859,7 +1859,7 @@
       <c r="H26" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="47"/>
+      <c r="I26" s="38"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -1872,13 +1872,13 @@
       <c r="S26" s="3"/>
     </row>
     <row r="27" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="43" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="25" t="s">
@@ -1892,7 +1892,7 @@
       <c r="H27" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I27" s="45" t="s">
+      <c r="I27" s="36" t="s">
         <v>11</v>
       </c>
       <c r="J27" s="3"/>
@@ -1907,9 +1907,9 @@
       <c r="S27" s="3"/>
     </row>
     <row r="28" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="43"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="22" t="s">
         <v>32</v>
       </c>
@@ -1921,7 +1921,7 @@
       <c r="H28" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="I28" s="46"/>
+      <c r="I28" s="37"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -1934,9 +1934,9 @@
       <c r="S28" s="3"/>
     </row>
     <row r="29" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="43"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="22" t="s">
         <v>52</v>
       </c>
@@ -1948,7 +1948,7 @@
       <c r="H29" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="I29" s="46"/>
+      <c r="I29" s="37"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -1961,9 +1961,9 @@
       <c r="S29" s="3"/>
     </row>
     <row r="30" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="37"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="43"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="44"/>
       <c r="D30" s="21" t="s">
         <v>53</v>
       </c>
@@ -1975,7 +1975,7 @@
       <c r="H30" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="I30" s="46"/>
+      <c r="I30" s="37"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -1988,9 +1988,9 @@
       <c r="S30" s="3"/>
     </row>
     <row r="31" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="37"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="43"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="44"/>
       <c r="D31" s="20" t="s">
         <v>54</v>
       </c>
@@ -2002,7 +2002,7 @@
       <c r="H31" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="I31" s="46"/>
+      <c r="I31" s="37"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
@@ -2015,10 +2015,10 @@
       <c r="S31" s="3"/>
     </row>
     <row r="32" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="41" t="s">
         <v>50</v>
       </c>
       <c r="C32" s="59" t="s">
@@ -2031,7 +2031,7 @@
       <c r="F32" s="24"/>
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
-      <c r="I32" s="45" t="s">
+      <c r="I32" s="36" t="s">
         <v>11</v>
       </c>
       <c r="J32" s="3"/>
@@ -2046,8 +2046,8 @@
       <c r="S32" s="3"/>
     </row>
     <row r="33" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="37"/>
-      <c r="B33" s="40"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="42"/>
       <c r="C33" s="60"/>
       <c r="D33" s="29" t="s">
         <v>62</v>
@@ -2060,7 +2060,7 @@
       <c r="H33" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="I33" s="46"/>
+      <c r="I33" s="37"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
@@ -2073,8 +2073,8 @@
       <c r="S33" s="3"/>
     </row>
     <row r="34" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
-      <c r="B34" s="40"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="42"/>
       <c r="C34" s="60"/>
       <c r="D34" s="29" t="s">
         <v>63</v>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
-      <c r="I34" s="46"/>
+      <c r="I34" s="37"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
@@ -2098,8 +2098,8 @@
       <c r="S34" s="3"/>
     </row>
     <row r="35" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="37"/>
-      <c r="B35" s="40"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="42"/>
       <c r="C35" s="60"/>
       <c r="D35" s="30" t="s">
         <v>64</v>
@@ -2112,7 +2112,7 @@
       <c r="H35" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="I35" s="47"/>
+      <c r="I35" s="38"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -2125,14 +2125,14 @@
       <c r="S35" s="3"/>
     </row>
     <row r="36" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="42" t="s">
-        <v>76</v>
+      <c r="C36" s="43" t="s">
+        <v>84</v>
       </c>
       <c r="D36" s="25" t="s">
         <v>22</v>
@@ -2145,14 +2145,14 @@
       <c r="H36" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="45" t="s">
+      <c r="I36" s="36" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="37"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="43"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="44"/>
       <c r="D37" s="22" t="s">
         <v>32</v>
       </c>
@@ -2164,15 +2164,15 @@
       <c r="H37" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="I37" s="46"/>
+      <c r="I37" s="37"/>
       <c r="J37" s="3"/>
     </row>
     <row r="38" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="37"/>
-      <c r="B38" s="40"/>
-      <c r="C38" s="43"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="44"/>
       <c r="D38" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E38" s="17"/>
       <c r="F38" s="22"/>
@@ -2182,34 +2182,34 @@
       <c r="H38" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="I38" s="46"/>
+      <c r="I38" s="37"/>
       <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="37"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="43"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="44"/>
       <c r="D39" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="23"/>
       <c r="G39" s="21"/>
       <c r="H39" s="32"/>
-      <c r="I39" s="46"/>
+      <c r="I39" s="37"/>
     </row>
     <row r="40" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="37"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="43"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="44"/>
       <c r="D40" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
       <c r="H40" s="34"/>
-      <c r="I40" s="46"/>
+      <c r="I40" s="37"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
@@ -2222,19 +2222,19 @@
       <c r="S40" s="3"/>
     </row>
     <row r="41" spans="1:19" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="37"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="43"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="44"/>
       <c r="D41" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E41" s="17"/>
       <c r="F41" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G41" s="17"/>
       <c r="H41" s="34"/>
-      <c r="I41" s="46"/>
+      <c r="I41" s="37"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
@@ -2247,17 +2247,17 @@
       <c r="S41" s="3"/>
     </row>
     <row r="42" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="37"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="43"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="44"/>
       <c r="D42" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
       <c r="G42" s="17"/>
       <c r="H42" s="34"/>
-      <c r="I42" s="46"/>
+      <c r="I42" s="37"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
@@ -2270,21 +2270,21 @@
       <c r="S42" s="3"/>
     </row>
     <row r="43" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="38"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="44"/>
+      <c r="A43" s="45"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="58"/>
       <c r="D43" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E43" s="26"/>
       <c r="F43" s="26"/>
       <c r="G43" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H43" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="I43" s="47"/>
+        <v>83</v>
+      </c>
+      <c r="I43" s="38"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
@@ -8001,22 +8001,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="A36:A43"/>
     <mergeCell ref="B36:B43"/>
     <mergeCell ref="C36:C43"/>
@@ -8033,6 +8017,22 @@
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="C32:C35"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>